<commit_message>
fix zero inventory coveralls issues
</commit_message>
<xml_diff>
--- a/app/shiny/templates/template_dropshipment.xlsx
+++ b/app/shiny/templates/template_dropshipment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibrown\Documents\ppe\distribute_12-11-2020\next_cycle_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B98CA0-5F87-46C2-94FE-1A330E0664E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F930DCF-17C5-41CB-9777-436813F220FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="4575" windowWidth="15585" windowHeight="9735" xr2:uid="{923FFECB-4A25-480B-9F4B-77073757D37B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{923FFECB-4A25-480B-9F4B-77073757D37B}"/>
   </bookViews>
   <sheets>
     <sheet name="WA#_Agency" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
     <t>Delivered By:</t>
   </si>
   <si>
-    <t>Order Time: 12/11/2020</t>
+    <t>Order Time: 1/22/2021</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -239,11 +239,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -259,7 +266,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5A23C8D-B7C2-4941-A49F-2B3576CCCA85}" name="Table27" displayName="Table27" ref="A16:E21" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Line"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Line" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="Item"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="Quantity"/>
@@ -568,30 +575,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3FA63A-2A70-4AB1-86F6-D1E6A018A4A0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="49.1796875" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -599,7 +607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -607,7 +615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -615,7 +623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -623,7 +631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -631,7 +639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -639,7 +647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -650,14 +658,14 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
@@ -667,14 +675,14 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -691,8 +699,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
         <v>1</v>
       </c>
       <c r="B17" t="s">
@@ -708,8 +716,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
         <v>2</v>
       </c>
       <c r="B18" t="s">
@@ -725,8 +733,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="9">
         <v>3</v>
       </c>
       <c r="B19" t="s">
@@ -742,16 +750,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
         <v>4</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
         <v>5</v>
       </c>
     </row>

</xml_diff>